<commit_message>
Add Excel sheets regarding types
</commit_message>
<xml_diff>
--- a/Excels/Copy of Invoice_app_field_list.xlsx
+++ b/Excels/Copy of Invoice_app_field_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alext\Desktop\fiori-invoice oneDrive\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F81026D1-0E3B-43E6-BC72-2D7DAD4C268A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15669239-92B4-4B6D-8CAE-6EE5A190FDF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10155" yWindow="1050" windowWidth="12840" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -863,7 +863,7 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1820,6 +1820,7 @@
   <autoFilter ref="A1:G39" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>